<commit_message>
added footprint to giga schematic
</commit_message>
<xml_diff>
--- a/Arduino Pins.xlsx
+++ b/Arduino Pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sammy\Desktop\PCB Projects\Hamburger_PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C43848-B4BF-4DE2-B189-04FB123AD2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80EB35A-2EBB-4D1C-B6BD-EB126CFC9034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{7F292513-6691-4751-BE98-05AAF28D81C4}"/>
+    <workbookView xWindow="-20832" yWindow="-96" windowWidth="20928" windowHeight="12432" activeTab="3" xr2:uid="{7F292513-6691-4751-BE98-05AAF28D81C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Table015 (Page 16)" sheetId="3" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="141">
   <si>
     <t>Pin</t>
   </si>
@@ -490,6 +490,9 @@
   </si>
   <si>
     <t>Digital Pins (D22-D53)</t>
+  </si>
+  <si>
+    <t>Input</t>
   </si>
 </sst>
 </file>
@@ -525,9 +528,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,9 +685,9 @@
   <autoFilter ref="A1:D19" xr:uid="{8130D3B2-5C6A-4FB1-8C6C-6B9D7283C84E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{036F0D48-1510-40D4-B15E-44B659EAD7D7}" uniqueName="1" name="Pin" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{1B9BA9B3-8741-454E-A44B-B4314149EE11}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{FBCCB06D-C660-49F6-B0C1-7A65624873F3}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{3A0D6DA4-88EA-488D-BF3F-386BF259ABB0}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{1B9BA9B3-8741-454E-A44B-B4314149EE11}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{FBCCB06D-C660-49F6-B0C1-7A65624873F3}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{3A0D6DA4-88EA-488D-BF3F-386BF259ABB0}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -696,9 +698,9 @@
   <autoFilter ref="A1:D27" xr:uid="{D85C6AEC-EEF2-4984-B902-878770199BAD}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{75CC5539-EE00-40E5-A3D6-BF6679697741}" uniqueName="1" name="Pin" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{12A07D9E-CB3E-4C3E-8FC8-29BC1179F9C6}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{45EA6D13-125D-4120-9FD6-5A93C45BDF75}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{E5D1E702-626A-42F0-ADBD-941D2070E520}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{12A07D9E-CB3E-4C3E-8FC8-29BC1179F9C6}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{45EA6D13-125D-4120-9FD6-5A93C45BDF75}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{E5D1E702-626A-42F0-ADBD-941D2070E520}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -709,9 +711,9 @@
   <autoFilter ref="A1:D25" xr:uid="{CEB35A60-BAF5-4A69-A62E-40BE845A8ABB}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B957ECF1-EE8A-4889-A6CB-42F6F53F80E6}" uniqueName="1" name="Pin" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{30C6E9A7-49A2-46BE-BFAE-1C5D0DD57A3D}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{DDF0B144-027B-4F96-AEB0-C961414A4A51}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{A06ED88F-3FD8-4350-B3AA-B1369D6A007D}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{30C6E9A7-49A2-46BE-BFAE-1C5D0DD57A3D}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{DDF0B144-027B-4F96-AEB0-C961414A4A51}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{A06ED88F-3FD8-4350-B3AA-B1369D6A007D}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -722,9 +724,9 @@
   <autoFilter ref="A2:D28" xr:uid="{467127DF-8B7F-47ED-8C45-066D504D10B6}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{406A33CE-2A58-41B6-87D8-D28424769CA7}" uniqueName="1" name="Pin" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{36FA58E4-81AA-450D-9684-6FDD3393BBB2}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{A64E08AD-8379-4B70-9657-A621878E755A}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{38DE2F16-CC87-4095-8393-ECD9629E0BF3}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{36FA58E4-81AA-450D-9684-6FDD3393BBB2}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{A64E08AD-8379-4B70-9657-A621878E755A}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{38DE2F16-CC87-4095-8393-ECD9629E0BF3}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -735,9 +737,9 @@
   <autoFilter ref="G2:J20" xr:uid="{305CD6DF-8A44-4273-957E-E6979CBA39D8}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C6E1720F-211C-47A6-B04E-7EF28533E91D}" uniqueName="1" name="Pin" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{C94BE149-3976-48AE-866A-BE887C049877}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{ADFBB25B-22FE-4BE1-B530-1260052F12E1}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{921CD8B3-CC85-48CA-996C-FA1C716FD391}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{C94BE149-3976-48AE-866A-BE887C049877}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{ADFBB25B-22FE-4BE1-B530-1260052F12E1}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{921CD8B3-CC85-48CA-996C-FA1C716FD391}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1079,15 +1081,15 @@
       <selection sqref="A1:D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.89453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.89453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1101,255 +1103,255 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>84</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>86</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>90</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1369,16 +1371,16 @@
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="5.89453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.20703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1392,367 +1394,367 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="1" t="s">
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="1" t="s">
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="1" t="s">
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1772,15 +1774,15 @@
       <selection sqref="A1:D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.89453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.1015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1794,339 +1796,339 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>102</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>104</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>102</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>106</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>102</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>102</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>110</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>102</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>112</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>102</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>114</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>102</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>102</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>118</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>120</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>102</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>122</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>102</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>124</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>102</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>126</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>102</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>128</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>102</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>130</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>132</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2142,18 +2144,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2370ABD-EF40-410E-9290-87B3F9AEBB14}">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3:O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="4" max="4" width="39.5546875" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" customWidth="1"/>
-    <col min="16" max="16" width="38.109375" customWidth="1"/>
+    <col min="4" max="4" width="39.5234375" customWidth="1"/>
+    <col min="10" max="10" width="13.5234375" customWidth="1"/>
+    <col min="16" max="16" width="38.1015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>138</v>
       </c>
@@ -2164,7 +2166,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2202,871 +2204,871 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" t="s">
         <v>59</v>
       </c>
       <c r="M3">
         <v>1</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" t="s">
         <v>92</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" t="s">
         <v>92</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J4" s="1" t="s">
+      <c r="I4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J4" t="s">
         <v>61</v>
       </c>
       <c r="M4">
         <v>2</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" t="s">
         <v>94</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="P4" s="1" t="s">
+      <c r="O4" t="s">
+        <v>134</v>
+      </c>
+      <c r="P4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="C5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="G5">
         <v>3</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" t="s">
         <v>62</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="I5" t="s">
+        <v>134</v>
+      </c>
+      <c r="J5" t="s">
         <v>63</v>
       </c>
       <c r="M5">
         <v>3</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" t="s">
         <v>96</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" t="s">
+        <v>140</v>
+      </c>
+      <c r="P5" t="s">
         <v>96</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>13</v>
       </c>
       <c r="G6">
         <v>4</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" t="s">
         <v>64</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J6" s="1" t="s">
+      <c r="I6" t="s">
+        <v>134</v>
+      </c>
+      <c r="J6" t="s">
         <v>65</v>
       </c>
       <c r="M6">
         <v>4</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="N6" t="s">
         <v>97</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="O6" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="C7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D7" t="s">
         <v>15</v>
       </c>
       <c r="G7">
         <v>5</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" t="s">
         <v>66</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="I7" t="s">
+        <v>134</v>
+      </c>
+      <c r="J7" t="s">
         <v>67</v>
       </c>
       <c r="M7">
         <v>5</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" t="s">
         <v>58</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" t="s">
         <v>12</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="C8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" t="s">
         <v>17</v>
       </c>
       <c r="G8">
         <v>6</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" t="s">
         <v>68</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J8" s="1" t="s">
+      <c r="I8" t="s">
+        <v>134</v>
+      </c>
+      <c r="J8" t="s">
         <v>69</v>
       </c>
       <c r="M8">
         <v>6</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N8" t="s">
         <v>11</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" t="s">
         <v>12</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
       </c>
       <c r="G9">
         <v>7</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" t="s">
         <v>70</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J9" s="1" t="s">
+      <c r="I9" t="s">
+        <v>134</v>
+      </c>
+      <c r="J9" t="s">
         <v>71</v>
       </c>
       <c r="M9">
         <v>7</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="N9" t="s">
         <v>11</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O9" t="s">
         <v>12</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="P9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="C10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" t="s">
         <v>21</v>
       </c>
       <c r="G10">
         <v>8</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" t="s">
         <v>72</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J10" s="1" t="s">
+      <c r="I10" t="s">
+        <v>134</v>
+      </c>
+      <c r="J10" t="s">
         <v>73</v>
       </c>
       <c r="M10">
         <v>8</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="N10" t="s">
         <v>99</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="O10" t="s">
         <v>12</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="P10" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="C11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" t="s">
         <v>23</v>
       </c>
       <c r="G11">
         <v>9</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" t="s">
         <v>74</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="I11" t="s">
+        <v>134</v>
+      </c>
+      <c r="J11" t="s">
         <v>75</v>
       </c>
       <c r="M11">
         <v>9</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="N11" t="s">
         <v>101</v>
       </c>
-      <c r="O11" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="P11" s="1" t="s">
+      <c r="O11" t="s">
+        <v>134</v>
+      </c>
+      <c r="P11" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="C12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" t="s">
         <v>25</v>
       </c>
       <c r="G12">
         <v>10</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" t="s">
         <v>76</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J12" s="1" t="s">
+      <c r="I12" t="s">
+        <v>134</v>
+      </c>
+      <c r="J12" t="s">
         <v>77</v>
       </c>
       <c r="M12">
         <v>10</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="N12" t="s">
         <v>104</v>
       </c>
-      <c r="O12" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="P12" s="1" t="s">
+      <c r="O12" t="s">
+        <v>134</v>
+      </c>
+      <c r="P12" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="C13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" t="s">
         <v>27</v>
       </c>
       <c r="G13">
         <v>11</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" t="s">
         <v>78</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J13" s="1" t="s">
+      <c r="I13" t="s">
+        <v>134</v>
+      </c>
+      <c r="J13" t="s">
         <v>79</v>
       </c>
       <c r="M13">
         <v>11</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="N13" t="s">
         <v>106</v>
       </c>
-      <c r="O13" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="P13" s="1" t="s">
+      <c r="O13" t="s">
+        <v>134</v>
+      </c>
+      <c r="P13" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="C14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14" t="s">
         <v>29</v>
       </c>
       <c r="G14">
         <v>12</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" t="s">
         <v>80</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J14" s="1" t="s">
+      <c r="I14" t="s">
+        <v>134</v>
+      </c>
+      <c r="J14" t="s">
         <v>81</v>
       </c>
       <c r="M14">
         <v>12</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="N14" t="s">
         <v>108</v>
       </c>
-      <c r="O14" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="P14" s="1" t="s">
+      <c r="O14" t="s">
+        <v>134</v>
+      </c>
+      <c r="P14" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="C15" t="s">
+        <v>134</v>
+      </c>
+      <c r="D15" t="s">
         <v>31</v>
       </c>
       <c r="G15">
         <v>13</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" t="s">
         <v>82</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J15" s="1" t="s">
+      <c r="I15" t="s">
+        <v>134</v>
+      </c>
+      <c r="J15" t="s">
         <v>83</v>
       </c>
       <c r="M15">
         <v>13</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="N15" t="s">
         <v>110</v>
       </c>
-      <c r="O15" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="P15" s="1" t="s">
+      <c r="O15" t="s">
+        <v>134</v>
+      </c>
+      <c r="P15" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="C16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" t="s">
         <v>33</v>
       </c>
       <c r="G16">
         <v>14</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" t="s">
         <v>84</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J16" s="1" t="s">
+      <c r="I16" t="s">
+        <v>134</v>
+      </c>
+      <c r="J16" t="s">
         <v>85</v>
       </c>
       <c r="M16">
         <v>14</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="N16" t="s">
         <v>112</v>
       </c>
-      <c r="O16" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="P16" s="1" t="s">
+      <c r="O16" t="s">
+        <v>134</v>
+      </c>
+      <c r="P16" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="C17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" t="s">
         <v>35</v>
       </c>
       <c r="G17">
         <v>15</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" t="s">
         <v>86</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J17" s="1" t="s">
+      <c r="I17" t="s">
+        <v>134</v>
+      </c>
+      <c r="J17" t="s">
         <v>87</v>
       </c>
       <c r="M17">
         <v>15</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="N17" t="s">
         <v>114</v>
       </c>
-      <c r="O17" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="P17" s="1" t="s">
+      <c r="O17" t="s">
+        <v>134</v>
+      </c>
+      <c r="P17" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="C18" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" t="s">
         <v>37</v>
       </c>
       <c r="G18">
         <v>16</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" t="s">
         <v>88</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J18" s="1" t="s">
+      <c r="I18" t="s">
+        <v>134</v>
+      </c>
+      <c r="J18" t="s">
         <v>89</v>
       </c>
       <c r="M18">
         <v>16</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="N18" t="s">
         <v>116</v>
       </c>
-      <c r="O18" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="P18" s="1" t="s">
+      <c r="O18" t="s">
+        <v>134</v>
+      </c>
+      <c r="P18" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="C19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19" t="s">
         <v>39</v>
       </c>
       <c r="G19">
         <v>17</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" t="s">
         <v>90</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J19" s="1" t="s">
+      <c r="I19" t="s">
+        <v>134</v>
+      </c>
+      <c r="J19" t="s">
         <v>91</v>
       </c>
       <c r="M19">
         <v>17</v>
       </c>
-      <c r="N19" s="1" t="s">
+      <c r="N19" t="s">
         <v>118</v>
       </c>
-      <c r="O19" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="P19" s="1" t="s">
+      <c r="O19" t="s">
+        <v>134</v>
+      </c>
+      <c r="P19" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="C20" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" t="s">
         <v>41</v>
       </c>
       <c r="G20">
         <v>18</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="I20" t="s">
         <v>12</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" t="s">
         <v>13</v>
       </c>
       <c r="M20">
         <v>18</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="N20" t="s">
         <v>120</v>
       </c>
-      <c r="O20" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="P20" s="1" t="s">
+      <c r="O20" t="s">
+        <v>134</v>
+      </c>
+      <c r="P20" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D21" s="1" t="s">
+      <c r="C21" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" t="s">
         <v>43</v>
       </c>
       <c r="M21">
         <v>19</v>
       </c>
-      <c r="N21" s="1" t="s">
+      <c r="N21" t="s">
         <v>122</v>
       </c>
-      <c r="O21" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="P21" s="1" t="s">
+      <c r="O21" t="s">
+        <v>134</v>
+      </c>
+      <c r="P21" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D22" s="1" t="s">
+      <c r="C22" t="s">
+        <v>134</v>
+      </c>
+      <c r="D22" t="s">
         <v>45</v>
       </c>
       <c r="M22">
         <v>20</v>
       </c>
-      <c r="N22" s="1" t="s">
+      <c r="N22" t="s">
         <v>124</v>
       </c>
-      <c r="O22" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="P22" s="1" t="s">
+      <c r="O22" t="s">
+        <v>134</v>
+      </c>
+      <c r="P22" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D23" s="1" t="s">
+      <c r="C23" t="s">
+        <v>134</v>
+      </c>
+      <c r="D23" t="s">
         <v>47</v>
       </c>
       <c r="M23">
         <v>21</v>
       </c>
-      <c r="N23" s="1" t="s">
+      <c r="N23" t="s">
         <v>126</v>
       </c>
-      <c r="O23" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="P23" s="1" t="s">
+      <c r="O23" t="s">
+        <v>134</v>
+      </c>
+      <c r="P23" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="C24" t="s">
+        <v>134</v>
+      </c>
+      <c r="D24" t="s">
         <v>49</v>
       </c>
       <c r="M24">
         <v>22</v>
       </c>
-      <c r="N24" s="1" t="s">
+      <c r="N24" t="s">
         <v>128</v>
       </c>
-      <c r="O24" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="P24" s="1" t="s">
+      <c r="O24" t="s">
+        <v>134</v>
+      </c>
+      <c r="P24" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="C25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D25" t="s">
         <v>51</v>
       </c>
       <c r="M25">
         <v>23</v>
       </c>
-      <c r="N25" s="1" t="s">
+      <c r="N25" t="s">
         <v>130</v>
       </c>
-      <c r="O25" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="P25" s="1" t="s">
+      <c r="O25" t="s">
+        <v>134</v>
+      </c>
+      <c r="P25" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="C26" t="s">
+        <v>134</v>
+      </c>
+      <c r="D26" t="s">
         <v>53</v>
       </c>
       <c r="M26">
         <v>24</v>
       </c>
-      <c r="N26" s="1" t="s">
+      <c r="N26" t="s">
         <v>132</v>
       </c>
-      <c r="O26" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="P26" s="1" t="s">
+      <c r="O26" t="s">
+        <v>134</v>
+      </c>
+      <c r="P26" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="C27" t="s">
+        <v>134</v>
+      </c>
+      <c r="D27" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="C28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D28" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reworked the schematic to feature all pins and added some ground vias
</commit_message>
<xml_diff>
--- a/Arduino Pins.xlsx
+++ b/Arduino Pins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sammy\Desktop\PCB Projects\Hamburger_PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80EB35A-2EBB-4D1C-B6BD-EB126CFC9034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0679300B-562E-43B0-AED2-1D335943EAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20832" yWindow="-96" windowWidth="20928" windowHeight="12432" activeTab="3" xr2:uid="{7F292513-6691-4751-BE98-05AAF28D81C4}"/>
   </bookViews>
@@ -19,11 +19,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="3" hidden="1">Sheet1!$A$2:$D$28</definedName>
+    <definedName name="ExternalData_1" localSheetId="3" hidden="1">Sheet1!$A$2:$C$28</definedName>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Table013 (Page 15)'!$A$1:$D$27</definedName>
-    <definedName name="ExternalData_2" localSheetId="3" hidden="1">Sheet1!$G$2:$J$20</definedName>
+    <definedName name="ExternalData_2" localSheetId="3" hidden="1">Sheet1!$I$2:$K$38</definedName>
     <definedName name="ExternalData_2" localSheetId="0" hidden="1">'Table015 (Page 16)'!$A$1:$D$19</definedName>
-    <definedName name="ExternalData_3" localSheetId="3" hidden="1">Sheet1!$M$2:$P$26</definedName>
+    <definedName name="ExternalData_3" localSheetId="3" hidden="1">Sheet1!$P$2:$R$26</definedName>
     <definedName name="ExternalData_3" localSheetId="2" hidden="1">'Table012 (Page 14)'!$A$1:$D$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="219">
   <si>
     <t>Pin</t>
   </si>
@@ -493,13 +493,247 @@
   </si>
   <si>
     <t>Input</t>
+  </si>
+  <si>
+    <t>SCL1</t>
+  </si>
+  <si>
+    <t>SDA1</t>
+  </si>
+  <si>
+    <t>SCK</t>
+  </si>
+  <si>
+    <t>CIPO</t>
+  </si>
+  <si>
+    <t>COPI</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>TX0</t>
+  </si>
+  <si>
+    <t>TX3</t>
+  </si>
+  <si>
+    <t>RX3</t>
+  </si>
+  <si>
+    <t>TX2</t>
+  </si>
+  <si>
+    <t>RX2</t>
+  </si>
+  <si>
+    <t>TX1</t>
+  </si>
+  <si>
+    <t>RX1</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>Designator</t>
+  </si>
+  <si>
+    <t>Side</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>GND1</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>RX0</t>
+  </si>
+  <si>
+    <t>D0/RX0</t>
+  </si>
+  <si>
+    <t>D23</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>D25</t>
+  </si>
+  <si>
+    <t>D27</t>
+  </si>
+  <si>
+    <t>D29</t>
+  </si>
+  <si>
+    <t>D31</t>
+  </si>
+  <si>
+    <t>D33</t>
+  </si>
+  <si>
+    <t>D35</t>
+  </si>
+  <si>
+    <t>D37</t>
+  </si>
+  <si>
+    <t>D39</t>
+  </si>
+  <si>
+    <t>D41</t>
+  </si>
+  <si>
+    <t>D43</t>
+  </si>
+  <si>
+    <t>D45</t>
+  </si>
+  <si>
+    <t>D47</t>
+  </si>
+  <si>
+    <t>D49</t>
+  </si>
+  <si>
+    <t>D51</t>
+  </si>
+  <si>
+    <t>D53</t>
+  </si>
+  <si>
+    <t>Bottom</t>
+  </si>
+  <si>
+    <t>5V3</t>
+  </si>
+  <si>
+    <t>GND3</t>
+  </si>
+  <si>
+    <t>5V4</t>
+  </si>
+  <si>
+    <t>GND5</t>
+  </si>
+  <si>
+    <t>GND6</t>
+  </si>
+  <si>
+    <t>GPIO 23</t>
+  </si>
+  <si>
+    <t>GPIO 25</t>
+  </si>
+  <si>
+    <t>GPIO 27</t>
+  </si>
+  <si>
+    <t>GPIO 29</t>
+  </si>
+  <si>
+    <t>GPIO 31</t>
+  </si>
+  <si>
+    <t>GPIO 33</t>
+  </si>
+  <si>
+    <t>GPIO 35</t>
+  </si>
+  <si>
+    <t>GPIO 37</t>
+  </si>
+  <si>
+    <t>GPIO 39</t>
+  </si>
+  <si>
+    <t>GPIO 41</t>
+  </si>
+  <si>
+    <t>GPIO 43</t>
+  </si>
+  <si>
+    <t>GPIO 45</t>
+  </si>
+  <si>
+    <t>GPIO 47</t>
+  </si>
+  <si>
+    <t>GPIO 49</t>
+  </si>
+  <si>
+    <t>GPIO 51</t>
+  </si>
+  <si>
+    <t>GPIO 53</t>
+  </si>
+  <si>
+    <t>IORF</t>
+  </si>
+  <si>
+    <t>RST1</t>
+  </si>
+  <si>
+    <t>3V3</t>
+  </si>
+  <si>
+    <t>5V1</t>
+  </si>
+  <si>
+    <t>GND2</t>
+  </si>
+  <si>
+    <t>CANR</t>
+  </si>
+  <si>
+    <t>CANT</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>SPI</t>
+  </si>
+  <si>
+    <t>MISO</t>
+  </si>
+  <si>
+    <t>RST2</t>
+  </si>
+  <si>
+    <t>5V2</t>
+  </si>
+  <si>
+    <t>MOSI</t>
+  </si>
+  <si>
+    <t>GND4</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Top</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,16 +741,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -524,17 +784,78 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="24">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -643,39 +964,54 @@
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="4" xr16:uid="{03C5D7BD-B3CF-42C8-BB31-C3BB0B50BC0C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="5">
-    <queryTableFields count="4">
+  <queryTableRefresh nextId="7" unboundColumnsRight="3">
+    <queryTableFields count="6">
       <queryTableField id="1" name="Pin" tableColumnId="1"/>
       <queryTableField id="2" name="Function" tableColumnId="2"/>
       <queryTableField id="3" name="Type" tableColumnId="3"/>
-      <queryTableField id="4" name="Description" tableColumnId="4"/>
+      <queryTableField id="4" dataBound="0" tableColumnId="4"/>
+      <queryTableField id="5" dataBound="0" tableColumnId="5"/>
+      <queryTableField id="6" dataBound="0" tableColumnId="6"/>
     </queryTableFields>
+    <queryTableDeletedFields count="1">
+      <deletedField name="Description"/>
+    </queryTableDeletedFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_2" connectionId="6" xr16:uid="{C3A5F69A-4BB3-4F5A-9B28-8532D4BAA80E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="5">
-    <queryTableFields count="4">
+  <queryTableRefresh nextId="7" unboundColumnsRight="3">
+    <queryTableFields count="6">
       <queryTableField id="1" name="Pin" tableColumnId="1"/>
       <queryTableField id="2" name="Function" tableColumnId="2"/>
       <queryTableField id="3" name="Type" tableColumnId="3"/>
-      <queryTableField id="4" name="Description" tableColumnId="4"/>
+      <queryTableField id="4" dataBound="0" tableColumnId="4"/>
+      <queryTableField id="5" dataBound="0" tableColumnId="5"/>
+      <queryTableField id="6" dataBound="0" tableColumnId="6"/>
     </queryTableFields>
+    <queryTableDeletedFields count="1">
+      <deletedField name="Description"/>
+    </queryTableDeletedFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_3" connectionId="2" xr16:uid="{33E73B6F-C696-4943-9419-BD0709AAFBB8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="5">
-    <queryTableFields count="4">
+  <queryTableRefresh nextId="7" unboundColumnsRight="3">
+    <queryTableFields count="6">
       <queryTableField id="1" name="Pin" tableColumnId="1"/>
       <queryTableField id="2" name="Function" tableColumnId="2"/>
       <queryTableField id="3" name="Type" tableColumnId="3"/>
-      <queryTableField id="4" name="Description" tableColumnId="4"/>
+      <queryTableField id="4" dataBound="0" tableColumnId="4"/>
+      <queryTableField id="5" dataBound="0" tableColumnId="5"/>
+      <queryTableField id="6" dataBound="0" tableColumnId="6"/>
     </queryTableFields>
+    <queryTableDeletedFields count="1">
+      <deletedField name="Description"/>
+    </queryTableDeletedFields>
   </queryTableRefresh>
 </queryTable>
 </file>
@@ -685,9 +1021,9 @@
   <autoFilter ref="A1:D19" xr:uid="{8130D3B2-5C6A-4FB1-8C6C-6B9D7283C84E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{036F0D48-1510-40D4-B15E-44B659EAD7D7}" uniqueName="1" name="Pin" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{1B9BA9B3-8741-454E-A44B-B4314149EE11}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{FBCCB06D-C660-49F6-B0C1-7A65624873F3}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{3A0D6DA4-88EA-488D-BF3F-386BF259ABB0}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{1B9BA9B3-8741-454E-A44B-B4314149EE11}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{FBCCB06D-C660-49F6-B0C1-7A65624873F3}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{3A0D6DA4-88EA-488D-BF3F-386BF259ABB0}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -698,9 +1034,9 @@
   <autoFilter ref="A1:D27" xr:uid="{D85C6AEC-EEF2-4984-B902-878770199BAD}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{75CC5539-EE00-40E5-A3D6-BF6679697741}" uniqueName="1" name="Pin" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{12A07D9E-CB3E-4C3E-8FC8-29BC1179F9C6}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{45EA6D13-125D-4120-9FD6-5A93C45BDF75}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{E5D1E702-626A-42F0-ADBD-941D2070E520}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{12A07D9E-CB3E-4C3E-8FC8-29BC1179F9C6}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{45EA6D13-125D-4120-9FD6-5A93C45BDF75}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{E5D1E702-626A-42F0-ADBD-941D2070E520}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -711,48 +1047,54 @@
   <autoFilter ref="A1:D25" xr:uid="{CEB35A60-BAF5-4A69-A62E-40BE845A8ABB}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B957ECF1-EE8A-4889-A6CB-42F6F53F80E6}" uniqueName="1" name="Pin" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{30C6E9A7-49A2-46BE-BFAE-1C5D0DD57A3D}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{DDF0B144-027B-4F96-AEB0-C961414A4A51}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{A06ED88F-3FD8-4350-B3AA-B1369D6A007D}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{30C6E9A7-49A2-46BE-BFAE-1C5D0DD57A3D}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{DDF0B144-027B-4F96-AEB0-C961414A4A51}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{A06ED88F-3FD8-4350-B3AA-B1369D6A007D}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{467127DF-8B7F-47ED-8C45-066D504D10B6}" name="Table013__Page_155" displayName="Table013__Page_155" ref="A2:D28" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A2:D28" xr:uid="{467127DF-8B7F-47ED-8C45-066D504D10B6}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{467127DF-8B7F-47ED-8C45-066D504D10B6}" name="Table013__Page_155" displayName="Table013__Page_155" ref="A2:F28" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A2:F28" xr:uid="{467127DF-8B7F-47ED-8C45-066D504D10B6}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{406A33CE-2A58-41B6-87D8-D28424769CA7}" uniqueName="1" name="Pin" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{36FA58E4-81AA-450D-9684-6FDD3393BBB2}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{A64E08AD-8379-4B70-9657-A621878E755A}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{38DE2F16-CC87-4095-8393-ECD9629E0BF3}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{36FA58E4-81AA-450D-9684-6FDD3393BBB2}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{A64E08AD-8379-4B70-9657-A621878E755A}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{38DE2F16-CC87-4095-8393-ECD9629E0BF3}" uniqueName="4" name="Designator" queryTableFieldId="4" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{CFF70E1B-CBCC-4320-B42F-44F9F908E975}" uniqueName="5" name="Side" queryTableFieldId="5" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{38702B71-C54D-427B-B613-54F55751ABBC}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{305CD6DF-8A44-4273-957E-E6979CBA39D8}" name="Table015__Page_166" displayName="Table015__Page_166" ref="G2:J20" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="G2:J20" xr:uid="{305CD6DF-8A44-4273-957E-E6979CBA39D8}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{305CD6DF-8A44-4273-957E-E6979CBA39D8}" name="Table015__Page_166" displayName="Table015__Page_166" ref="I2:N38" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="I2:N38" xr:uid="{305CD6DF-8A44-4273-957E-E6979CBA39D8}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{C6E1720F-211C-47A6-B04E-7EF28533E91D}" uniqueName="1" name="Pin" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{C94BE149-3976-48AE-866A-BE887C049877}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{ADFBB25B-22FE-4BE1-B530-1260052F12E1}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{921CD8B3-CC85-48CA-996C-FA1C716FD391}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{C94BE149-3976-48AE-866A-BE887C049877}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{ADFBB25B-22FE-4BE1-B530-1260052F12E1}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{921CD8B3-CC85-48CA-996C-FA1C716FD391}" uniqueName="4" name="Designator" queryTableFieldId="4" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{69528022-1446-4BDE-959A-72248D380D64}" uniqueName="5" name="Side" queryTableFieldId="5" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{60C9919B-0510-4960-BE3A-E96FD4D66B35}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B7481E4B-B4E8-4EDE-82B8-41A9E329473F}" name="Table012__Page_148" displayName="Table012__Page_148" ref="M2:P26" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="M2:P26" xr:uid="{B7481E4B-B4E8-4EDE-82B8-41A9E329473F}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B7481E4B-B4E8-4EDE-82B8-41A9E329473F}" name="Table012__Page_148" displayName="Table012__Page_148" ref="P2:U26" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="P2:U26" xr:uid="{B7481E4B-B4E8-4EDE-82B8-41A9E329473F}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{398460D7-E406-41C4-B41E-9122A532B9D9}" uniqueName="1" name="Pin" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{3F530B70-2AAC-49CC-A7FC-3EBF2F3F396A}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{10835939-CD2D-486C-B727-CE453821B75F}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{42E72A7C-EFC3-41D4-A857-8F54D1EC8BEC}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{3F530B70-2AAC-49CC-A7FC-3EBF2F3F396A}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{10835939-CD2D-486C-B727-CE453821B75F}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{42E72A7C-EFC3-41D4-A857-8F54D1EC8BEC}" uniqueName="4" name="Designator" queryTableFieldId="4" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{15B6FDCD-B690-44C4-89FE-CE9A6D955101}" uniqueName="5" name="Side" queryTableFieldId="5" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{F963A267-951A-4BFF-BD22-2C9582B7CBF0}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1081,15 +1423,15 @@
       <selection sqref="A1:D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.89453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.41796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.1015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.89453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1103,7 +1445,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1117,7 +1459,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1131,7 +1473,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1145,7 +1487,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1159,7 +1501,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1173,7 +1515,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1187,7 +1529,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1201,7 +1543,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1215,7 +1557,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1229,7 +1571,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1243,7 +1585,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1257,7 +1599,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1271,7 +1613,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1285,7 +1627,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1299,7 +1641,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1313,7 +1655,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1327,7 +1669,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1341,7 +1683,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1371,16 +1713,16 @@
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.89453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.41796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.1015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.20703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.89453125" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1394,7 +1736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1408,7 +1750,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1422,7 +1764,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1436,7 +1778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1450,7 +1792,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1464,7 +1806,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1478,7 +1820,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1492,7 +1834,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1506,7 +1848,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1520,7 +1862,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1534,7 +1876,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1548,7 +1890,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1562,7 +1904,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1576,7 +1918,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1590,7 +1932,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1604,7 +1946,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1618,7 +1960,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1632,7 +1974,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1646,7 +1988,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1660,7 +2002,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1674,7 +2016,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1688,7 +2030,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1702,7 +2044,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1716,7 +2058,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1730,7 +2072,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1744,7 +2086,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1774,15 +2116,15 @@
       <selection sqref="A1:D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.89453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.41796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.1015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.1015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1796,7 +2138,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1810,7 +2152,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1824,7 +2166,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1838,7 +2180,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1852,7 +2194,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1866,7 +2208,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1880,7 +2222,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1894,7 +2236,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1908,7 +2250,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1922,7 +2264,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1936,7 +2278,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1950,7 +2292,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1964,7 +2306,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1978,7 +2320,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1992,7 +2334,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2006,7 +2348,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2020,7 +2362,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2034,7 +2376,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2048,7 +2390,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2062,7 +2404,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2076,7 +2418,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2090,7 +2432,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2104,7 +2446,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2118,7 +2460,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2142,31 +2484,37 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2370ABD-EF40-410E-9290-87B3F9AEBB14}">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:O3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="39.5234375" customWidth="1"/>
-    <col min="10" max="10" width="13.5234375" customWidth="1"/>
-    <col min="16" max="16" width="38.1015625" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" customWidth="1"/>
+    <col min="6" max="6" width="41.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" customWidth="1"/>
+    <col min="14" max="14" width="15" customWidth="1"/>
+    <col min="16" max="16" width="10.5546875" customWidth="1"/>
+    <col min="19" max="19" width="10.77734375" customWidth="1"/>
+    <col min="21" max="21" width="37.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>138</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>139</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2177,34 +2525,52 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>1</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>2</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
+        <v>156</v>
+      </c>
+      <c r="M2" t="s">
+        <v>157</v>
+      </c>
+      <c r="N2" t="s">
         <v>3</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>0</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
         <v>1</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" t="s">
         <v>2</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" t="s">
+        <v>156</v>
+      </c>
+      <c r="T2" t="s">
+        <v>157</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2215,34 +2581,52 @@
         <v>134</v>
       </c>
       <c r="D3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
+        <v>165</v>
+      </c>
+      <c r="K3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
+        <v>182</v>
+      </c>
+      <c r="M3" t="s">
+        <v>181</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="M3">
+      <c r="P3">
         <v>1</v>
       </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>92</v>
       </c>
-      <c r="O3" t="s">
+      <c r="R3" t="s">
         <v>92</v>
       </c>
-      <c r="P3" t="s">
+      <c r="S3" t="s">
+        <v>92</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U3" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2253,34 +2637,50 @@
         <v>134</v>
       </c>
       <c r="D4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>2</v>
       </c>
-      <c r="H4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I4" t="s">
-        <v>134</v>
-      </c>
-      <c r="J4" t="s">
-        <v>61</v>
-      </c>
-      <c r="M4">
+      <c r="J4" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="M4" t="s">
+        <v>181</v>
+      </c>
+      <c r="N4" s="4"/>
+      <c r="P4">
         <v>2</v>
       </c>
-      <c r="N4" t="s">
+      <c r="Q4" t="s">
         <v>94</v>
       </c>
-      <c r="O4" t="s">
-        <v>134</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
+        <v>134</v>
+      </c>
+      <c r="S4" t="s">
+        <v>203</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U4" s="6" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2291,34 +2691,52 @@
         <v>134</v>
       </c>
       <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>3</v>
       </c>
-      <c r="H5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I5" t="s">
-        <v>134</v>
-      </c>
       <c r="J5" t="s">
-        <v>63</v>
-      </c>
-      <c r="M5">
+        <v>60</v>
+      </c>
+      <c r="K5" t="s">
+        <v>134</v>
+      </c>
+      <c r="L5" t="s">
+        <v>60</v>
+      </c>
+      <c r="M5" t="s">
+        <v>181</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="P5">
         <v>3</v>
       </c>
-      <c r="N5" t="s">
+      <c r="Q5" t="s">
         <v>96</v>
       </c>
-      <c r="O5" t="s">
+      <c r="R5" t="s">
         <v>140</v>
       </c>
-      <c r="P5" t="s">
+      <c r="S5" t="s">
+        <v>204</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U5" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2329,34 +2747,52 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>4</v>
       </c>
-      <c r="H6" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" t="s">
-        <v>134</v>
-      </c>
       <c r="J6" t="s">
-        <v>65</v>
-      </c>
-      <c r="M6">
+        <v>164</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="M6" t="s">
+        <v>181</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="P6">
         <v>4</v>
       </c>
-      <c r="N6" t="s">
+      <c r="Q6" t="s">
         <v>97</v>
       </c>
-      <c r="O6" t="s">
+      <c r="R6" t="s">
         <v>12</v>
       </c>
-      <c r="P6" t="s">
+      <c r="S6" t="s">
+        <v>205</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U6" s="6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2367,34 +2803,52 @@
         <v>134</v>
       </c>
       <c r="D7" t="s">
+        <v>143</v>
+      </c>
+      <c r="E7" t="s">
+        <v>158</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7" t="s">
-        <v>66</v>
-      </c>
-      <c r="I7" t="s">
-        <v>134</v>
+      <c r="I7">
+        <v>5</v>
       </c>
       <c r="J7" t="s">
-        <v>67</v>
-      </c>
-      <c r="M7">
-        <v>5</v>
-      </c>
-      <c r="N7" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" t="s">
+        <v>134</v>
+      </c>
+      <c r="L7" t="s">
+        <v>62</v>
+      </c>
+      <c r="M7" t="s">
+        <v>181</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="P7">
+        <v>5</v>
+      </c>
+      <c r="Q7" t="s">
         <v>58</v>
       </c>
-      <c r="O7" t="s">
+      <c r="R7" t="s">
         <v>12</v>
       </c>
-      <c r="P7" t="s">
+      <c r="S7" t="s">
+        <v>206</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U7" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2405,34 +2859,52 @@
         <v>134</v>
       </c>
       <c r="D8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" t="s">
+        <v>158</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>6</v>
       </c>
-      <c r="H8" t="s">
-        <v>68</v>
-      </c>
-      <c r="I8" t="s">
-        <v>134</v>
-      </c>
       <c r="J8" t="s">
-        <v>69</v>
-      </c>
-      <c r="M8">
+        <v>166</v>
+      </c>
+      <c r="K8" t="s">
+        <v>134</v>
+      </c>
+      <c r="L8" t="s">
+        <v>166</v>
+      </c>
+      <c r="M8" t="s">
+        <v>181</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="P8">
         <v>6</v>
       </c>
-      <c r="N8" t="s">
+      <c r="Q8" t="s">
         <v>11</v>
       </c>
-      <c r="O8" t="s">
+      <c r="R8" t="s">
         <v>12</v>
       </c>
-      <c r="P8" t="s">
+      <c r="S8" t="s">
+        <v>207</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U8" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2443,34 +2915,52 @@
         <v>134</v>
       </c>
       <c r="D9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" t="s">
+        <v>158</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>7</v>
       </c>
-      <c r="H9" t="s">
-        <v>70</v>
-      </c>
-      <c r="I9" t="s">
-        <v>134</v>
-      </c>
       <c r="J9" t="s">
-        <v>71</v>
-      </c>
-      <c r="M9">
+        <v>64</v>
+      </c>
+      <c r="K9" t="s">
+        <v>134</v>
+      </c>
+      <c r="L9" t="s">
+        <v>64</v>
+      </c>
+      <c r="M9" t="s">
+        <v>181</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="P9">
         <v>7</v>
       </c>
-      <c r="N9" t="s">
+      <c r="Q9" t="s">
         <v>11</v>
       </c>
-      <c r="O9" t="s">
+      <c r="R9" t="s">
         <v>12</v>
       </c>
-      <c r="P9" t="s">
+      <c r="S9" t="s">
+        <v>183</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U9" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2481,34 +2971,52 @@
         <v>134</v>
       </c>
       <c r="D10" t="s">
+        <v>146</v>
+      </c>
+      <c r="E10" t="s">
+        <v>158</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>8</v>
       </c>
-      <c r="H10" t="s">
-        <v>72</v>
-      </c>
-      <c r="I10" t="s">
-        <v>134</v>
-      </c>
       <c r="J10" t="s">
-        <v>73</v>
-      </c>
-      <c r="M10">
+        <v>167</v>
+      </c>
+      <c r="K10" t="s">
+        <v>134</v>
+      </c>
+      <c r="L10" t="s">
+        <v>167</v>
+      </c>
+      <c r="M10" t="s">
+        <v>181</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="P10">
         <v>8</v>
       </c>
-      <c r="N10" t="s">
+      <c r="Q10" t="s">
         <v>99</v>
       </c>
-      <c r="O10" t="s">
+      <c r="R10" t="s">
         <v>12</v>
       </c>
-      <c r="P10" t="s">
+      <c r="S10" t="s">
+        <v>99</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U10" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2519,34 +3027,52 @@
         <v>134</v>
       </c>
       <c r="D11" t="s">
+        <v>160</v>
+      </c>
+      <c r="E11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>9</v>
       </c>
-      <c r="H11" t="s">
-        <v>74</v>
-      </c>
-      <c r="I11" t="s">
-        <v>134</v>
-      </c>
       <c r="J11" t="s">
-        <v>75</v>
-      </c>
-      <c r="M11">
+        <v>66</v>
+      </c>
+      <c r="K11" t="s">
+        <v>134</v>
+      </c>
+      <c r="L11" t="s">
+        <v>66</v>
+      </c>
+      <c r="M11" t="s">
+        <v>181</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="P11">
         <v>9</v>
       </c>
-      <c r="N11" t="s">
+      <c r="Q11" t="s">
         <v>101</v>
       </c>
-      <c r="O11" t="s">
-        <v>134</v>
-      </c>
-      <c r="P11" t="s">
+      <c r="R11" t="s">
+        <v>134</v>
+      </c>
+      <c r="S11" t="s">
+        <v>101</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U11" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2557,34 +3083,52 @@
         <v>134</v>
       </c>
       <c r="D12" t="s">
+        <v>161</v>
+      </c>
+      <c r="E12" t="s">
+        <v>158</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>10</v>
       </c>
-      <c r="H12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I12" t="s">
-        <v>134</v>
-      </c>
       <c r="J12" t="s">
-        <v>77</v>
-      </c>
-      <c r="M12">
+        <v>168</v>
+      </c>
+      <c r="K12" t="s">
+        <v>134</v>
+      </c>
+      <c r="L12" t="s">
+        <v>168</v>
+      </c>
+      <c r="M12" t="s">
+        <v>181</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="P12">
         <v>10</v>
       </c>
-      <c r="N12" t="s">
+      <c r="Q12" t="s">
         <v>104</v>
       </c>
-      <c r="O12" t="s">
-        <v>134</v>
-      </c>
-      <c r="P12" t="s">
+      <c r="R12" t="s">
+        <v>134</v>
+      </c>
+      <c r="S12" t="s">
+        <v>104</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U12" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2595,34 +3139,52 @@
         <v>134</v>
       </c>
       <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>158</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <v>11</v>
       </c>
-      <c r="H13" t="s">
-        <v>78</v>
-      </c>
-      <c r="I13" t="s">
-        <v>134</v>
-      </c>
       <c r="J13" t="s">
-        <v>79</v>
-      </c>
-      <c r="M13">
+        <v>68</v>
+      </c>
+      <c r="K13" t="s">
+        <v>134</v>
+      </c>
+      <c r="L13" t="s">
+        <v>68</v>
+      </c>
+      <c r="M13" t="s">
+        <v>181</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="P13">
         <v>11</v>
       </c>
-      <c r="N13" t="s">
+      <c r="Q13" t="s">
         <v>106</v>
       </c>
-      <c r="O13" t="s">
-        <v>134</v>
-      </c>
-      <c r="P13" t="s">
+      <c r="R13" t="s">
+        <v>134</v>
+      </c>
+      <c r="S13" t="s">
+        <v>106</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U13" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2633,34 +3195,52 @@
         <v>134</v>
       </c>
       <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>158</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G14">
+      <c r="I14">
         <v>12</v>
       </c>
-      <c r="H14" t="s">
-        <v>80</v>
-      </c>
-      <c r="I14" t="s">
-        <v>134</v>
-      </c>
       <c r="J14" t="s">
-        <v>81</v>
-      </c>
-      <c r="M14">
+        <v>169</v>
+      </c>
+      <c r="K14" t="s">
+        <v>134</v>
+      </c>
+      <c r="L14" t="s">
+        <v>169</v>
+      </c>
+      <c r="M14" t="s">
+        <v>181</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="P14">
         <v>12</v>
       </c>
-      <c r="N14" t="s">
+      <c r="Q14" t="s">
         <v>108</v>
       </c>
-      <c r="O14" t="s">
-        <v>134</v>
-      </c>
-      <c r="P14" t="s">
+      <c r="R14" t="s">
+        <v>134</v>
+      </c>
+      <c r="S14" t="s">
+        <v>108</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U14" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2671,34 +3251,52 @@
         <v>134</v>
       </c>
       <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" t="s">
+        <v>158</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G15">
+      <c r="I15">
         <v>13</v>
       </c>
-      <c r="H15" t="s">
-        <v>82</v>
-      </c>
-      <c r="I15" t="s">
-        <v>134</v>
-      </c>
       <c r="J15" t="s">
-        <v>83</v>
-      </c>
-      <c r="M15">
+        <v>70</v>
+      </c>
+      <c r="K15" t="s">
+        <v>134</v>
+      </c>
+      <c r="L15" t="s">
+        <v>70</v>
+      </c>
+      <c r="M15" t="s">
+        <v>181</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P15">
         <v>13</v>
       </c>
-      <c r="N15" t="s">
+      <c r="Q15" t="s">
         <v>110</v>
       </c>
-      <c r="O15" t="s">
-        <v>134</v>
-      </c>
-      <c r="P15" t="s">
+      <c r="R15" t="s">
+        <v>134</v>
+      </c>
+      <c r="S15" t="s">
+        <v>110</v>
+      </c>
+      <c r="T15" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U15" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2709,34 +3307,52 @@
         <v>134</v>
       </c>
       <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" t="s">
+        <v>158</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G16">
+      <c r="I16">
         <v>14</v>
       </c>
-      <c r="H16" t="s">
-        <v>84</v>
-      </c>
-      <c r="I16" t="s">
-        <v>134</v>
-      </c>
       <c r="J16" t="s">
-        <v>85</v>
-      </c>
-      <c r="M16">
+        <v>170</v>
+      </c>
+      <c r="K16" t="s">
+        <v>134</v>
+      </c>
+      <c r="L16" t="s">
+        <v>170</v>
+      </c>
+      <c r="M16" t="s">
+        <v>181</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="P16">
         <v>14</v>
       </c>
-      <c r="N16" t="s">
+      <c r="Q16" t="s">
         <v>112</v>
       </c>
-      <c r="O16" t="s">
-        <v>134</v>
-      </c>
-      <c r="P16" t="s">
+      <c r="R16" t="s">
+        <v>134</v>
+      </c>
+      <c r="S16" t="s">
+        <v>112</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U16" s="6" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2747,34 +3363,52 @@
         <v>134</v>
       </c>
       <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
+        <v>158</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G17">
+      <c r="I17">
         <v>15</v>
       </c>
-      <c r="H17" t="s">
-        <v>86</v>
-      </c>
-      <c r="I17" t="s">
-        <v>134</v>
-      </c>
       <c r="J17" t="s">
-        <v>87</v>
-      </c>
-      <c r="M17">
+        <v>72</v>
+      </c>
+      <c r="K17" t="s">
+        <v>134</v>
+      </c>
+      <c r="L17" t="s">
+        <v>72</v>
+      </c>
+      <c r="M17" t="s">
+        <v>181</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="P17">
         <v>15</v>
       </c>
-      <c r="N17" t="s">
+      <c r="Q17" t="s">
         <v>114</v>
       </c>
-      <c r="O17" t="s">
-        <v>134</v>
-      </c>
-      <c r="P17" t="s">
+      <c r="R17" t="s">
+        <v>134</v>
+      </c>
+      <c r="S17" t="s">
+        <v>114</v>
+      </c>
+      <c r="T17" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U17" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2785,34 +3419,52 @@
         <v>134</v>
       </c>
       <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G18">
+      <c r="I18">
         <v>16</v>
       </c>
-      <c r="H18" t="s">
-        <v>88</v>
-      </c>
-      <c r="I18" t="s">
-        <v>134</v>
-      </c>
       <c r="J18" t="s">
-        <v>89</v>
-      </c>
-      <c r="M18">
+        <v>171</v>
+      </c>
+      <c r="K18" t="s">
+        <v>134</v>
+      </c>
+      <c r="L18" t="s">
+        <v>171</v>
+      </c>
+      <c r="M18" t="s">
+        <v>181</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="P18">
         <v>16</v>
       </c>
-      <c r="N18" t="s">
+      <c r="Q18" t="s">
         <v>116</v>
       </c>
-      <c r="O18" t="s">
-        <v>134</v>
-      </c>
-      <c r="P18" t="s">
+      <c r="R18" t="s">
+        <v>134</v>
+      </c>
+      <c r="S18" t="s">
+        <v>116</v>
+      </c>
+      <c r="T18" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U18" s="6" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2823,72 +3475,108 @@
         <v>134</v>
       </c>
       <c r="D19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E19" t="s">
+        <v>158</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G19">
+      <c r="I19">
         <v>17</v>
       </c>
-      <c r="H19" t="s">
-        <v>90</v>
-      </c>
-      <c r="I19" t="s">
-        <v>134</v>
-      </c>
       <c r="J19" t="s">
-        <v>91</v>
-      </c>
-      <c r="M19">
+        <v>74</v>
+      </c>
+      <c r="K19" t="s">
+        <v>134</v>
+      </c>
+      <c r="L19" t="s">
+        <v>74</v>
+      </c>
+      <c r="M19" t="s">
+        <v>181</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="P19">
         <v>17</v>
       </c>
-      <c r="N19" t="s">
+      <c r="Q19" t="s">
         <v>118</v>
       </c>
-      <c r="O19" t="s">
-        <v>134</v>
-      </c>
-      <c r="P19" t="s">
+      <c r="R19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S19" t="s">
+        <v>118</v>
+      </c>
+      <c r="T19" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U19" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>163</v>
       </c>
       <c r="C20" t="s">
         <v>134</v>
       </c>
       <c r="D20" t="s">
+        <v>162</v>
+      </c>
+      <c r="E20" t="s">
+        <v>158</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G20">
+      <c r="I20">
         <v>18</v>
       </c>
-      <c r="H20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" t="s">
-        <v>12</v>
-      </c>
       <c r="J20" t="s">
-        <v>13</v>
-      </c>
-      <c r="M20">
+        <v>172</v>
+      </c>
+      <c r="K20" t="s">
+        <v>134</v>
+      </c>
+      <c r="L20" t="s">
+        <v>172</v>
+      </c>
+      <c r="M20" t="s">
+        <v>181</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="P20">
         <v>18</v>
       </c>
-      <c r="N20" t="s">
+      <c r="Q20" t="s">
         <v>120</v>
       </c>
-      <c r="O20" t="s">
-        <v>134</v>
-      </c>
-      <c r="P20" t="s">
+      <c r="R20" t="s">
+        <v>134</v>
+      </c>
+      <c r="S20" t="s">
+        <v>120</v>
+      </c>
+      <c r="T20" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U20" s="6" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2899,22 +3587,52 @@
         <v>134</v>
       </c>
       <c r="D21" t="s">
+        <v>148</v>
+      </c>
+      <c r="E21" t="s">
+        <v>158</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="M21">
+      <c r="I21">
         <v>19</v>
       </c>
-      <c r="N21" t="s">
+      <c r="J21" t="s">
+        <v>76</v>
+      </c>
+      <c r="K21" t="s">
+        <v>134</v>
+      </c>
+      <c r="L21" t="s">
+        <v>76</v>
+      </c>
+      <c r="M21" t="s">
+        <v>181</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="P21">
+        <v>19</v>
+      </c>
+      <c r="Q21" t="s">
         <v>122</v>
       </c>
-      <c r="O21" t="s">
-        <v>134</v>
-      </c>
-      <c r="P21" t="s">
+      <c r="R21" t="s">
+        <v>134</v>
+      </c>
+      <c r="S21" t="s">
+        <v>122</v>
+      </c>
+      <c r="T21" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U21" s="5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2925,22 +3643,52 @@
         <v>134</v>
       </c>
       <c r="D22" t="s">
+        <v>149</v>
+      </c>
+      <c r="E22" t="s">
+        <v>158</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="M22">
+      <c r="I22">
         <v>20</v>
       </c>
-      <c r="N22" t="s">
+      <c r="J22" t="s">
+        <v>173</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L22" t="s">
+        <v>173</v>
+      </c>
+      <c r="M22" t="s">
+        <v>181</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="P22">
+        <v>20</v>
+      </c>
+      <c r="Q22" t="s">
         <v>124</v>
       </c>
-      <c r="O22" t="s">
-        <v>134</v>
-      </c>
-      <c r="P22" t="s">
+      <c r="R22" t="s">
+        <v>134</v>
+      </c>
+      <c r="S22" t="s">
+        <v>124</v>
+      </c>
+      <c r="T22" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U22" s="6" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2951,22 +3699,52 @@
         <v>134</v>
       </c>
       <c r="D23" t="s">
+        <v>150</v>
+      </c>
+      <c r="E23" t="s">
+        <v>158</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="M23">
+      <c r="I23">
         <v>21</v>
       </c>
-      <c r="N23" t="s">
+      <c r="J23" t="s">
+        <v>78</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L23" t="s">
+        <v>78</v>
+      </c>
+      <c r="M23" t="s">
+        <v>181</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="P23">
+        <v>21</v>
+      </c>
+      <c r="Q23" t="s">
         <v>126</v>
       </c>
-      <c r="O23" t="s">
-        <v>134</v>
-      </c>
-      <c r="P23" t="s">
+      <c r="R23" t="s">
+        <v>134</v>
+      </c>
+      <c r="S23" t="s">
+        <v>126</v>
+      </c>
+      <c r="T23" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U23" s="5" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2977,22 +3755,52 @@
         <v>134</v>
       </c>
       <c r="D24" t="s">
+        <v>151</v>
+      </c>
+      <c r="E24" t="s">
+        <v>158</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="M24">
+      <c r="I24">
         <v>22</v>
       </c>
-      <c r="N24" t="s">
+      <c r="J24" t="s">
+        <v>174</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L24" t="s">
+        <v>174</v>
+      </c>
+      <c r="M24" t="s">
+        <v>181</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="P24">
+        <v>22</v>
+      </c>
+      <c r="Q24" t="s">
         <v>128</v>
       </c>
-      <c r="O24" t="s">
-        <v>134</v>
-      </c>
-      <c r="P24" t="s">
+      <c r="R24" t="s">
+        <v>134</v>
+      </c>
+      <c r="S24" t="s">
+        <v>128</v>
+      </c>
+      <c r="T24" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U24" s="6" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3003,22 +3811,52 @@
         <v>134</v>
       </c>
       <c r="D25" t="s">
+        <v>152</v>
+      </c>
+      <c r="E25" t="s">
+        <v>158</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="M25">
+      <c r="I25">
         <v>23</v>
       </c>
-      <c r="N25" t="s">
+      <c r="J25" t="s">
+        <v>80</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L25" t="s">
+        <v>80</v>
+      </c>
+      <c r="M25" t="s">
+        <v>181</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="P25">
+        <v>23</v>
+      </c>
+      <c r="Q25" t="s">
         <v>130</v>
       </c>
-      <c r="O25" t="s">
-        <v>134</v>
-      </c>
-      <c r="P25" t="s">
+      <c r="R25" t="s">
+        <v>134</v>
+      </c>
+      <c r="S25" t="s">
+        <v>208</v>
+      </c>
+      <c r="T25" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U25" s="5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -3029,22 +3867,52 @@
         <v>134</v>
       </c>
       <c r="D26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E26" t="s">
+        <v>158</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="M26">
+      <c r="I26">
         <v>24</v>
       </c>
-      <c r="N26" t="s">
+      <c r="J26" t="s">
+        <v>175</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L26" t="s">
+        <v>175</v>
+      </c>
+      <c r="M26" t="s">
+        <v>181</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="P26">
+        <v>24</v>
+      </c>
+      <c r="Q26" t="s">
         <v>132</v>
       </c>
-      <c r="O26" t="s">
-        <v>134</v>
-      </c>
-      <c r="P26" t="s">
+      <c r="R26" t="s">
+        <v>134</v>
+      </c>
+      <c r="S26" t="s">
+        <v>209</v>
+      </c>
+      <c r="T26" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U26" s="6" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3055,10 +3923,34 @@
         <v>134</v>
       </c>
       <c r="D27" t="s">
+        <v>154</v>
+      </c>
+      <c r="E27" t="s">
+        <v>158</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="I27">
+        <v>25</v>
+      </c>
+      <c r="J27" t="s">
+        <v>82</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L27" t="s">
+        <v>82</v>
+      </c>
+      <c r="M27" t="s">
+        <v>181</v>
+      </c>
+      <c r="N27" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3069,10 +3961,346 @@
         <v>134</v>
       </c>
       <c r="D28" t="s">
+        <v>155</v>
+      </c>
+      <c r="E28" t="s">
+        <v>158</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="I28">
+        <v>26</v>
+      </c>
+      <c r="J28" t="s">
+        <v>176</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L28" t="s">
+        <v>176</v>
+      </c>
+      <c r="M28" t="s">
+        <v>181</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="I29">
+        <v>27</v>
+      </c>
+      <c r="J29" t="s">
+        <v>84</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L29" t="s">
+        <v>84</v>
+      </c>
+      <c r="M29" t="s">
+        <v>181</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>211</v>
+      </c>
+      <c r="I30">
+        <v>28</v>
+      </c>
+      <c r="J30" t="s">
+        <v>177</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L30" t="s">
+        <v>177</v>
+      </c>
+      <c r="M30" t="s">
+        <v>181</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I31">
+        <v>29</v>
+      </c>
+      <c r="J31" t="s">
+        <v>86</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L31" t="s">
+        <v>86</v>
+      </c>
+      <c r="M31" t="s">
+        <v>181</v>
+      </c>
+      <c r="N31" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>212</v>
+      </c>
+      <c r="C32" t="s">
+        <v>140</v>
+      </c>
+      <c r="D32" t="s">
+        <v>212</v>
+      </c>
+      <c r="E32" t="s">
+        <v>218</v>
+      </c>
+      <c r="I32">
+        <v>30</v>
+      </c>
+      <c r="J32" t="s">
+        <v>178</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L32" t="s">
+        <v>178</v>
+      </c>
+      <c r="M32" t="s">
+        <v>181</v>
+      </c>
+      <c r="N32" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" t="s">
+        <v>217</v>
+      </c>
+      <c r="D33" t="s">
+        <v>143</v>
+      </c>
+      <c r="E33" t="s">
+        <v>218</v>
+      </c>
+      <c r="I33">
+        <v>31</v>
+      </c>
+      <c r="J33" t="s">
+        <v>88</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L33" t="s">
+        <v>88</v>
+      </c>
+      <c r="M33" t="s">
+        <v>181</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>213</v>
+      </c>
+      <c r="C34" t="s">
+        <v>140</v>
+      </c>
+      <c r="D34" t="s">
+        <v>213</v>
+      </c>
+      <c r="E34" t="s">
+        <v>218</v>
+      </c>
+      <c r="I34">
+        <v>32</v>
+      </c>
+      <c r="J34" t="s">
+        <v>179</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L34" t="s">
+        <v>179</v>
+      </c>
+      <c r="M34" t="s">
+        <v>181</v>
+      </c>
+      <c r="N34" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>214</v>
+      </c>
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" t="s">
+        <v>214</v>
+      </c>
+      <c r="E35" t="s">
+        <v>218</v>
+      </c>
+      <c r="I35">
+        <v>33</v>
+      </c>
+      <c r="J35" t="s">
+        <v>90</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L35" t="s">
+        <v>90</v>
+      </c>
+      <c r="M35" t="s">
+        <v>181</v>
+      </c>
+      <c r="N35" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>215</v>
+      </c>
+      <c r="C36" t="s">
+        <v>217</v>
+      </c>
+      <c r="D36" t="s">
+        <v>215</v>
+      </c>
+      <c r="E36" t="s">
+        <v>218</v>
+      </c>
+      <c r="I36">
+        <v>34</v>
+      </c>
+      <c r="J36" t="s">
+        <v>180</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L36" t="s">
+        <v>180</v>
+      </c>
+      <c r="M36" t="s">
+        <v>181</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>216</v>
+      </c>
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" t="s">
+        <v>216</v>
+      </c>
+      <c r="E37" t="s">
+        <v>218</v>
+      </c>
+      <c r="I37">
+        <v>35</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="M37" t="s">
+        <v>181</v>
+      </c>
+      <c r="N37" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I38">
+        <v>36</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="N38" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="3">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
added SD card slots and 4-layers
</commit_message>
<xml_diff>
--- a/Arduino Pins.xlsx
+++ b/Arduino Pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sammy\Desktop\PCB Projects\Hamburger_PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0679300B-562E-43B0-AED2-1D335943EAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD035449-3402-4FF1-B190-8A393467E217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20832" yWindow="-96" windowWidth="20928" windowHeight="12432" activeTab="3" xr2:uid="{7F292513-6691-4751-BE98-05AAF28D81C4}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" activeTab="3" xr2:uid="{7F292513-6691-4751-BE98-05AAF28D81C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Table015 (Page 16)" sheetId="3" r:id="rId1"/>
@@ -825,14 +825,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1063,8 +1062,8 @@
     <tableColumn id="2" xr3:uid="{36FA58E4-81AA-450D-9684-6FDD3393BBB2}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="14"/>
     <tableColumn id="3" xr3:uid="{A64E08AD-8379-4B70-9657-A621878E755A}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="13"/>
     <tableColumn id="4" xr3:uid="{38DE2F16-CC87-4095-8393-ECD9629E0BF3}" uniqueName="4" name="Designator" queryTableFieldId="4" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{CFF70E1B-CBCC-4320-B42F-44F9F908E975}" uniqueName="5" name="Side" queryTableFieldId="5" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{38702B71-C54D-427B-B613-54F55751ABBC}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{CFF70E1B-CBCC-4320-B42F-44F9F908E975}" uniqueName="5" name="Side" queryTableFieldId="5" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{38702B71-C54D-427B-B613-54F55751ABBC}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1075,11 +1074,11 @@
   <autoFilter ref="I2:N38" xr:uid="{305CD6DF-8A44-4273-957E-E6979CBA39D8}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{C6E1720F-211C-47A6-B04E-7EF28533E91D}" uniqueName="1" name="Pin" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{C94BE149-3976-48AE-866A-BE887C049877}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{ADFBB25B-22FE-4BE1-B530-1260052F12E1}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{921CD8B3-CC85-48CA-996C-FA1C716FD391}" uniqueName="4" name="Designator" queryTableFieldId="4" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{69528022-1446-4BDE-959A-72248D380D64}" uniqueName="5" name="Side" queryTableFieldId="5" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{60C9919B-0510-4960-BE3A-E96FD4D66B35}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{C94BE149-3976-48AE-866A-BE887C049877}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{ADFBB25B-22FE-4BE1-B530-1260052F12E1}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{921CD8B3-CC85-48CA-996C-FA1C716FD391}" uniqueName="4" name="Designator" queryTableFieldId="4" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{69528022-1446-4BDE-959A-72248D380D64}" uniqueName="5" name="Side" queryTableFieldId="5" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{60C9919B-0510-4960-BE3A-E96FD4D66B35}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1090,9 +1089,9 @@
   <autoFilter ref="P2:U26" xr:uid="{B7481E4B-B4E8-4EDE-82B8-41A9E329473F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{398460D7-E406-41C4-B41E-9122A532B9D9}" uniqueName="1" name="Pin" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{3F530B70-2AAC-49CC-A7FC-3EBF2F3F396A}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{10835939-CD2D-486C-B727-CE453821B75F}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{42E72A7C-EFC3-41D4-A857-8F54D1EC8BEC}" uniqueName="4" name="Designator" queryTableFieldId="4" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{3F530B70-2AAC-49CC-A7FC-3EBF2F3F396A}" uniqueName="2" name="Function" queryTableFieldId="2" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{10835939-CD2D-486C-B727-CE453821B75F}" uniqueName="3" name="Type" queryTableFieldId="3" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{42E72A7C-EFC3-41D4-A857-8F54D1EC8BEC}" uniqueName="4" name="Designator" queryTableFieldId="4" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{15B6FDCD-B690-44C4-89FE-CE9A6D955101}" uniqueName="5" name="Side" queryTableFieldId="5" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{F963A267-951A-4BFF-BD22-2C9582B7CBF0}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="0"/>
   </tableColumns>
@@ -1423,15 +1422,15 @@
       <selection sqref="A1:D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.89453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.89453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1445,7 +1444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1459,7 +1458,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1473,7 +1472,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1487,7 +1486,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1501,7 +1500,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1515,7 +1514,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1529,7 +1528,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1543,7 +1542,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1557,7 +1556,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1571,7 +1570,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1585,7 +1584,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1599,7 +1598,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1613,7 +1612,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1627,7 +1626,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1641,7 +1640,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1655,7 +1654,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1669,7 +1668,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1683,7 +1682,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1713,16 +1712,16 @@
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="5.89453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.20703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1736,7 +1735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1750,7 +1749,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1764,7 +1763,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1778,7 +1777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1792,7 +1791,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1806,7 +1805,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1820,7 +1819,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1834,7 +1833,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1848,7 +1847,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1862,7 +1861,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1876,7 +1875,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1890,7 +1889,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1904,7 +1903,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1918,7 +1917,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1932,7 +1931,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1946,7 +1945,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1960,7 +1959,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1974,7 +1973,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1988,7 +1987,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2002,7 +2001,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2016,7 +2015,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2030,7 +2029,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2044,7 +2043,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2058,7 +2057,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2072,7 +2071,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2086,7 +2085,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2116,15 +2115,15 @@
       <selection sqref="A1:D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.89453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.1015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2138,7 +2137,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2152,7 +2151,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2166,7 +2165,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2180,7 +2179,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2194,7 +2193,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2208,7 +2207,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2222,7 +2221,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2236,7 +2235,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2250,7 +2249,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2264,7 +2263,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2278,7 +2277,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2292,7 +2291,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2306,7 +2305,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2320,7 +2319,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2334,7 +2333,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2348,7 +2347,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2362,7 +2361,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2376,7 +2375,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2390,7 +2389,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2404,7 +2403,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2418,7 +2417,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2432,7 +2431,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2446,7 +2445,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2460,7 +2459,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2486,24 +2485,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2370ABD-EF40-410E-9290-87B3F9AEBB14}">
   <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="9.44140625" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" customWidth="1"/>
-    <col min="5" max="5" width="19.88671875" customWidth="1"/>
-    <col min="6" max="6" width="41.6640625" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="9.41796875" customWidth="1"/>
+    <col min="4" max="4" width="12.7890625" customWidth="1"/>
+    <col min="5" max="5" width="19.89453125" customWidth="1"/>
+    <col min="6" max="6" width="41.68359375" customWidth="1"/>
+    <col min="10" max="10" width="13.5234375" customWidth="1"/>
     <col min="14" max="14" width="15" customWidth="1"/>
-    <col min="16" max="16" width="10.5546875" customWidth="1"/>
-    <col min="19" max="19" width="10.77734375" customWidth="1"/>
-    <col min="21" max="21" width="37.21875" customWidth="1"/>
+    <col min="16" max="16" width="10.5234375" customWidth="1"/>
+    <col min="19" max="19" width="10.7890625" customWidth="1"/>
+    <col min="21" max="21" width="37.20703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>138</v>
       </c>
@@ -2514,7 +2513,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2570,7 +2569,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2586,7 +2585,7 @@
       <c r="E3" t="s">
         <v>158</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
       <c r="I3">
@@ -2604,7 +2603,7 @@
       <c r="M3" t="s">
         <v>181</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" t="s">
         <v>59</v>
       </c>
       <c r="P3">
@@ -2619,14 +2618,14 @@
       <c r="S3" t="s">
         <v>92</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="T3" t="s">
         <v>210</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="U3" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2642,25 +2641,24 @@
       <c r="E4" t="s">
         <v>158</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" t="s">
         <v>8</v>
       </c>
       <c r="I4">
         <v>2</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" t="s">
         <v>165</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" t="s">
         <v>184</v>
       </c>
       <c r="M4" t="s">
         <v>181</v>
       </c>
-      <c r="N4" s="4"/>
       <c r="P4">
         <v>2</v>
       </c>
@@ -2673,14 +2671,14 @@
       <c r="S4" t="s">
         <v>203</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="T4" t="s">
         <v>210</v>
       </c>
-      <c r="U4" s="6" t="s">
+      <c r="U4" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2696,7 +2694,7 @@
       <c r="E5" t="s">
         <v>158</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" t="s">
         <v>10</v>
       </c>
       <c r="I5">
@@ -2714,7 +2712,7 @@
       <c r="M5" t="s">
         <v>181</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" t="s">
         <v>61</v>
       </c>
       <c r="P5">
@@ -2729,14 +2727,14 @@
       <c r="S5" t="s">
         <v>204</v>
       </c>
-      <c r="T5" s="4" t="s">
+      <c r="T5" t="s">
         <v>210</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="U5" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2752,7 +2750,7 @@
       <c r="E6" t="s">
         <v>158</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" t="s">
         <v>13</v>
       </c>
       <c r="I6">
@@ -2761,16 +2759,16 @@
       <c r="J6" t="s">
         <v>164</v>
       </c>
-      <c r="K6" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="L6" s="4" t="s">
+      <c r="K6" t="s">
+        <v>134</v>
+      </c>
+      <c r="L6" t="s">
         <v>164</v>
       </c>
       <c r="M6" t="s">
         <v>181</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="N6" t="s">
         <v>187</v>
       </c>
       <c r="P6">
@@ -2785,14 +2783,14 @@
       <c r="S6" t="s">
         <v>205</v>
       </c>
-      <c r="T6" s="4" t="s">
+      <c r="T6" t="s">
         <v>210</v>
       </c>
-      <c r="U6" s="6" t="s">
+      <c r="U6" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2808,7 +2806,7 @@
       <c r="E7" t="s">
         <v>158</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" t="s">
         <v>15</v>
       </c>
       <c r="I7">
@@ -2826,7 +2824,7 @@
       <c r="M7" t="s">
         <v>181</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="N7" t="s">
         <v>63</v>
       </c>
       <c r="P7">
@@ -2841,14 +2839,14 @@
       <c r="S7" t="s">
         <v>206</v>
       </c>
-      <c r="T7" s="4" t="s">
+      <c r="T7" t="s">
         <v>210</v>
       </c>
-      <c r="U7" s="5" t="s">
+      <c r="U7" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2864,7 +2862,7 @@
       <c r="E8" t="s">
         <v>158</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" t="s">
         <v>17</v>
       </c>
       <c r="I8">
@@ -2882,7 +2880,7 @@
       <c r="M8" t="s">
         <v>181</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" t="s">
         <v>188</v>
       </c>
       <c r="P8">
@@ -2897,14 +2895,14 @@
       <c r="S8" t="s">
         <v>207</v>
       </c>
-      <c r="T8" s="4" t="s">
+      <c r="T8" t="s">
         <v>210</v>
       </c>
-      <c r="U8" s="6" t="s">
+      <c r="U8" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2920,7 +2918,7 @@
       <c r="E9" t="s">
         <v>158</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" t="s">
         <v>19</v>
       </c>
       <c r="I9">
@@ -2938,7 +2936,7 @@
       <c r="M9" t="s">
         <v>181</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="N9" t="s">
         <v>65</v>
       </c>
       <c r="P9">
@@ -2953,14 +2951,14 @@
       <c r="S9" t="s">
         <v>183</v>
       </c>
-      <c r="T9" s="4" t="s">
+      <c r="T9" t="s">
         <v>210</v>
       </c>
-      <c r="U9" s="5" t="s">
+      <c r="U9" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2976,7 +2974,7 @@
       <c r="E10" t="s">
         <v>158</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" t="s">
         <v>21</v>
       </c>
       <c r="I10">
@@ -2994,7 +2992,7 @@
       <c r="M10" t="s">
         <v>181</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="N10" t="s">
         <v>189</v>
       </c>
       <c r="P10">
@@ -3009,14 +3007,14 @@
       <c r="S10" t="s">
         <v>99</v>
       </c>
-      <c r="T10" s="4" t="s">
+      <c r="T10" t="s">
         <v>210</v>
       </c>
-      <c r="U10" s="6" t="s">
+      <c r="U10" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3032,7 +3030,7 @@
       <c r="E11" t="s">
         <v>158</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" t="s">
         <v>23</v>
       </c>
       <c r="I11">
@@ -3050,7 +3048,7 @@
       <c r="M11" t="s">
         <v>181</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="N11" t="s">
         <v>67</v>
       </c>
       <c r="P11">
@@ -3065,14 +3063,14 @@
       <c r="S11" t="s">
         <v>101</v>
       </c>
-      <c r="T11" s="4" t="s">
+      <c r="T11" t="s">
         <v>210</v>
       </c>
-      <c r="U11" s="5" t="s">
+      <c r="U11" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3088,7 +3086,7 @@
       <c r="E12" t="s">
         <v>158</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" t="s">
         <v>25</v>
       </c>
       <c r="I12">
@@ -3106,7 +3104,7 @@
       <c r="M12" t="s">
         <v>181</v>
       </c>
-      <c r="N12" s="4" t="s">
+      <c r="N12" t="s">
         <v>190</v>
       </c>
       <c r="P12">
@@ -3121,14 +3119,14 @@
       <c r="S12" t="s">
         <v>104</v>
       </c>
-      <c r="T12" s="4" t="s">
+      <c r="T12" t="s">
         <v>210</v>
       </c>
-      <c r="U12" s="6" t="s">
+      <c r="U12" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3144,7 +3142,7 @@
       <c r="E13" t="s">
         <v>158</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" t="s">
         <v>27</v>
       </c>
       <c r="I13">
@@ -3162,7 +3160,7 @@
       <c r="M13" t="s">
         <v>181</v>
       </c>
-      <c r="N13" s="4" t="s">
+      <c r="N13" t="s">
         <v>69</v>
       </c>
       <c r="P13">
@@ -3177,14 +3175,14 @@
       <c r="S13" t="s">
         <v>106</v>
       </c>
-      <c r="T13" s="4" t="s">
+      <c r="T13" t="s">
         <v>210</v>
       </c>
-      <c r="U13" s="5" t="s">
+      <c r="U13" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3200,7 +3198,7 @@
       <c r="E14" t="s">
         <v>158</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" t="s">
         <v>29</v>
       </c>
       <c r="I14">
@@ -3218,7 +3216,7 @@
       <c r="M14" t="s">
         <v>181</v>
       </c>
-      <c r="N14" s="4" t="s">
+      <c r="N14" t="s">
         <v>191</v>
       </c>
       <c r="P14">
@@ -3233,14 +3231,14 @@
       <c r="S14" t="s">
         <v>108</v>
       </c>
-      <c r="T14" s="4" t="s">
+      <c r="T14" t="s">
         <v>210</v>
       </c>
-      <c r="U14" s="6" t="s">
+      <c r="U14" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3256,7 +3254,7 @@
       <c r="E15" t="s">
         <v>158</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" t="s">
         <v>31</v>
       </c>
       <c r="I15">
@@ -3274,7 +3272,7 @@
       <c r="M15" t="s">
         <v>181</v>
       </c>
-      <c r="N15" s="4" t="s">
+      <c r="N15" t="s">
         <v>71</v>
       </c>
       <c r="P15">
@@ -3289,14 +3287,14 @@
       <c r="S15" t="s">
         <v>110</v>
       </c>
-      <c r="T15" s="4" t="s">
+      <c r="T15" t="s">
         <v>210</v>
       </c>
-      <c r="U15" s="5" t="s">
+      <c r="U15" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3312,7 +3310,7 @@
       <c r="E16" t="s">
         <v>158</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" t="s">
         <v>33</v>
       </c>
       <c r="I16">
@@ -3330,7 +3328,7 @@
       <c r="M16" t="s">
         <v>181</v>
       </c>
-      <c r="N16" s="4" t="s">
+      <c r="N16" t="s">
         <v>192</v>
       </c>
       <c r="P16">
@@ -3345,14 +3343,14 @@
       <c r="S16" t="s">
         <v>112</v>
       </c>
-      <c r="T16" s="4" t="s">
+      <c r="T16" t="s">
         <v>210</v>
       </c>
-      <c r="U16" s="6" t="s">
+      <c r="U16" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3368,7 +3366,7 @@
       <c r="E17" t="s">
         <v>158</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" t="s">
         <v>35</v>
       </c>
       <c r="I17">
@@ -3386,7 +3384,7 @@
       <c r="M17" t="s">
         <v>181</v>
       </c>
-      <c r="N17" s="4" t="s">
+      <c r="N17" t="s">
         <v>73</v>
       </c>
       <c r="P17">
@@ -3401,14 +3399,14 @@
       <c r="S17" t="s">
         <v>114</v>
       </c>
-      <c r="T17" s="4" t="s">
+      <c r="T17" t="s">
         <v>210</v>
       </c>
-      <c r="U17" s="5" t="s">
+      <c r="U17" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3424,7 +3422,7 @@
       <c r="E18" t="s">
         <v>158</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" t="s">
         <v>37</v>
       </c>
       <c r="I18">
@@ -3442,7 +3440,7 @@
       <c r="M18" t="s">
         <v>181</v>
       </c>
-      <c r="N18" s="4" t="s">
+      <c r="N18" t="s">
         <v>193</v>
       </c>
       <c r="P18">
@@ -3457,14 +3455,14 @@
       <c r="S18" t="s">
         <v>116</v>
       </c>
-      <c r="T18" s="4" t="s">
+      <c r="T18" t="s">
         <v>210</v>
       </c>
-      <c r="U18" s="6" t="s">
+      <c r="U18" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>17</v>
       </c>
@@ -3480,7 +3478,7 @@
       <c r="E19" t="s">
         <v>158</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" t="s">
         <v>39</v>
       </c>
       <c r="I19">
@@ -3498,7 +3496,7 @@
       <c r="M19" t="s">
         <v>181</v>
       </c>
-      <c r="N19" s="4" t="s">
+      <c r="N19" t="s">
         <v>75</v>
       </c>
       <c r="P19">
@@ -3513,14 +3511,14 @@
       <c r="S19" t="s">
         <v>118</v>
       </c>
-      <c r="T19" s="4" t="s">
+      <c r="T19" t="s">
         <v>210</v>
       </c>
-      <c r="U19" s="5" t="s">
+      <c r="U19" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>18</v>
       </c>
@@ -3536,7 +3534,7 @@
       <c r="E20" t="s">
         <v>158</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" t="s">
         <v>41</v>
       </c>
       <c r="I20">
@@ -3554,7 +3552,7 @@
       <c r="M20" t="s">
         <v>181</v>
       </c>
-      <c r="N20" s="4" t="s">
+      <c r="N20" t="s">
         <v>194</v>
       </c>
       <c r="P20">
@@ -3569,14 +3567,14 @@
       <c r="S20" t="s">
         <v>120</v>
       </c>
-      <c r="T20" s="4" t="s">
+      <c r="T20" t="s">
         <v>210</v>
       </c>
-      <c r="U20" s="6" t="s">
+      <c r="U20" s="5" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>19</v>
       </c>
@@ -3592,7 +3590,7 @@
       <c r="E21" t="s">
         <v>158</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" t="s">
         <v>43</v>
       </c>
       <c r="I21">
@@ -3610,7 +3608,7 @@
       <c r="M21" t="s">
         <v>181</v>
       </c>
-      <c r="N21" s="4" t="s">
+      <c r="N21" t="s">
         <v>77</v>
       </c>
       <c r="P21">
@@ -3625,14 +3623,14 @@
       <c r="S21" t="s">
         <v>122</v>
       </c>
-      <c r="T21" s="4" t="s">
+      <c r="T21" t="s">
         <v>210</v>
       </c>
-      <c r="U21" s="5" t="s">
+      <c r="U21" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>20</v>
       </c>
@@ -3648,7 +3646,7 @@
       <c r="E22" t="s">
         <v>158</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" t="s">
         <v>45</v>
       </c>
       <c r="I22">
@@ -3657,7 +3655,7 @@
       <c r="J22" t="s">
         <v>173</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="K22" t="s">
         <v>134</v>
       </c>
       <c r="L22" t="s">
@@ -3666,7 +3664,7 @@
       <c r="M22" t="s">
         <v>181</v>
       </c>
-      <c r="N22" s="4" t="s">
+      <c r="N22" t="s">
         <v>195</v>
       </c>
       <c r="P22">
@@ -3681,14 +3679,14 @@
       <c r="S22" t="s">
         <v>124</v>
       </c>
-      <c r="T22" s="4" t="s">
+      <c r="T22" t="s">
         <v>210</v>
       </c>
-      <c r="U22" s="6" t="s">
+      <c r="U22" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>21</v>
       </c>
@@ -3704,7 +3702,7 @@
       <c r="E23" t="s">
         <v>158</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" t="s">
         <v>47</v>
       </c>
       <c r="I23">
@@ -3713,7 +3711,7 @@
       <c r="J23" t="s">
         <v>78</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="K23" t="s">
         <v>134</v>
       </c>
       <c r="L23" t="s">
@@ -3722,7 +3720,7 @@
       <c r="M23" t="s">
         <v>181</v>
       </c>
-      <c r="N23" s="4" t="s">
+      <c r="N23" t="s">
         <v>79</v>
       </c>
       <c r="P23">
@@ -3737,14 +3735,14 @@
       <c r="S23" t="s">
         <v>126</v>
       </c>
-      <c r="T23" s="4" t="s">
+      <c r="T23" t="s">
         <v>210</v>
       </c>
-      <c r="U23" s="5" t="s">
+      <c r="U23" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3760,7 +3758,7 @@
       <c r="E24" t="s">
         <v>158</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" t="s">
         <v>49</v>
       </c>
       <c r="I24">
@@ -3769,7 +3767,7 @@
       <c r="J24" t="s">
         <v>174</v>
       </c>
-      <c r="K24" s="4" t="s">
+      <c r="K24" t="s">
         <v>134</v>
       </c>
       <c r="L24" t="s">
@@ -3778,7 +3776,7 @@
       <c r="M24" t="s">
         <v>181</v>
       </c>
-      <c r="N24" s="4" t="s">
+      <c r="N24" t="s">
         <v>196</v>
       </c>
       <c r="P24">
@@ -3793,14 +3791,14 @@
       <c r="S24" t="s">
         <v>128</v>
       </c>
-      <c r="T24" s="4" t="s">
+      <c r="T24" t="s">
         <v>210</v>
       </c>
-      <c r="U24" s="6" t="s">
+      <c r="U24" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3816,7 +3814,7 @@
       <c r="E25" t="s">
         <v>158</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" t="s">
         <v>51</v>
       </c>
       <c r="I25">
@@ -3825,7 +3823,7 @@
       <c r="J25" t="s">
         <v>80</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="K25" t="s">
         <v>134</v>
       </c>
       <c r="L25" t="s">
@@ -3834,7 +3832,7 @@
       <c r="M25" t="s">
         <v>181</v>
       </c>
-      <c r="N25" s="4" t="s">
+      <c r="N25" t="s">
         <v>81</v>
       </c>
       <c r="P25">
@@ -3849,14 +3847,14 @@
       <c r="S25" t="s">
         <v>208</v>
       </c>
-      <c r="T25" s="4" t="s">
+      <c r="T25" t="s">
         <v>210</v>
       </c>
-      <c r="U25" s="5" t="s">
+      <c r="U25" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>24</v>
       </c>
@@ -3872,7 +3870,7 @@
       <c r="E26" t="s">
         <v>158</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" t="s">
         <v>53</v>
       </c>
       <c r="I26">
@@ -3881,7 +3879,7 @@
       <c r="J26" t="s">
         <v>175</v>
       </c>
-      <c r="K26" s="4" t="s">
+      <c r="K26" t="s">
         <v>134</v>
       </c>
       <c r="L26" t="s">
@@ -3890,7 +3888,7 @@
       <c r="M26" t="s">
         <v>181</v>
       </c>
-      <c r="N26" s="4" t="s">
+      <c r="N26" t="s">
         <v>197</v>
       </c>
       <c r="P26">
@@ -3905,14 +3903,14 @@
       <c r="S26" t="s">
         <v>209</v>
       </c>
-      <c r="T26" s="4" t="s">
+      <c r="T26" t="s">
         <v>210</v>
       </c>
-      <c r="U26" s="6" t="s">
+      <c r="U26" s="5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3928,7 +3926,7 @@
       <c r="E27" t="s">
         <v>158</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" t="s">
         <v>55</v>
       </c>
       <c r="I27">
@@ -3937,7 +3935,7 @@
       <c r="J27" t="s">
         <v>82</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="K27" t="s">
         <v>134</v>
       </c>
       <c r="L27" t="s">
@@ -3946,11 +3944,11 @@
       <c r="M27" t="s">
         <v>181</v>
       </c>
-      <c r="N27" s="4" t="s">
+      <c r="N27" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3966,7 +3964,7 @@
       <c r="E28" t="s">
         <v>158</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" t="s">
         <v>57</v>
       </c>
       <c r="I28">
@@ -3975,7 +3973,7 @@
       <c r="J28" t="s">
         <v>176</v>
       </c>
-      <c r="K28" s="4" t="s">
+      <c r="K28" t="s">
         <v>134</v>
       </c>
       <c r="L28" t="s">
@@ -3984,18 +3982,18 @@
       <c r="M28" t="s">
         <v>181</v>
       </c>
-      <c r="N28" s="4" t="s">
+      <c r="N28" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="I29">
         <v>27</v>
       </c>
       <c r="J29" t="s">
         <v>84</v>
       </c>
-      <c r="K29" s="4" t="s">
+      <c r="K29" t="s">
         <v>134</v>
       </c>
       <c r="L29" t="s">
@@ -4004,11 +4002,11 @@
       <c r="M29" t="s">
         <v>181</v>
       </c>
-      <c r="N29" s="4" t="s">
+      <c r="N29" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>211</v>
       </c>
@@ -4018,7 +4016,7 @@
       <c r="J30" t="s">
         <v>177</v>
       </c>
-      <c r="K30" s="4" t="s">
+      <c r="K30" t="s">
         <v>134</v>
       </c>
       <c r="L30" t="s">
@@ -4027,11 +4025,11 @@
       <c r="M30" t="s">
         <v>181</v>
       </c>
-      <c r="N30" s="4" t="s">
+      <c r="N30" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -4056,7 +4054,7 @@
       <c r="J31" t="s">
         <v>86</v>
       </c>
-      <c r="K31" s="4" t="s">
+      <c r="K31" t="s">
         <v>134</v>
       </c>
       <c r="L31" t="s">
@@ -4065,11 +4063,11 @@
       <c r="M31" t="s">
         <v>181</v>
       </c>
-      <c r="N31" s="4" t="s">
+      <c r="N31" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>1</v>
       </c>
@@ -4091,7 +4089,7 @@
       <c r="J32" t="s">
         <v>178</v>
       </c>
-      <c r="K32" s="4" t="s">
+      <c r="K32" t="s">
         <v>134</v>
       </c>
       <c r="L32" t="s">
@@ -4100,11 +4098,11 @@
       <c r="M32" t="s">
         <v>181</v>
       </c>
-      <c r="N32" s="4" t="s">
+      <c r="N32" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>2</v>
       </c>
@@ -4126,7 +4124,7 @@
       <c r="J33" t="s">
         <v>88</v>
       </c>
-      <c r="K33" s="4" t="s">
+      <c r="K33" t="s">
         <v>134</v>
       </c>
       <c r="L33" t="s">
@@ -4135,11 +4133,11 @@
       <c r="M33" t="s">
         <v>181</v>
       </c>
-      <c r="N33" s="4" t="s">
+      <c r="N33" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>3</v>
       </c>
@@ -4161,7 +4159,7 @@
       <c r="J34" t="s">
         <v>179</v>
       </c>
-      <c r="K34" s="4" t="s">
+      <c r="K34" t="s">
         <v>134</v>
       </c>
       <c r="L34" t="s">
@@ -4170,11 +4168,11 @@
       <c r="M34" t="s">
         <v>181</v>
       </c>
-      <c r="N34" s="4" t="s">
+      <c r="N34" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>4</v>
       </c>
@@ -4196,7 +4194,7 @@
       <c r="J35" t="s">
         <v>90</v>
       </c>
-      <c r="K35" s="4" t="s">
+      <c r="K35" t="s">
         <v>134</v>
       </c>
       <c r="L35" t="s">
@@ -4205,11 +4203,11 @@
       <c r="M35" t="s">
         <v>181</v>
       </c>
-      <c r="N35" s="4" t="s">
+      <c r="N35" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>5</v>
       </c>
@@ -4231,7 +4229,7 @@
       <c r="J36" t="s">
         <v>180</v>
       </c>
-      <c r="K36" s="4" t="s">
+      <c r="K36" t="s">
         <v>134</v>
       </c>
       <c r="L36" t="s">
@@ -4240,11 +4238,11 @@
       <c r="M36" t="s">
         <v>181</v>
       </c>
-      <c r="N36" s="4" t="s">
+      <c r="N36" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>6</v>
       </c>
@@ -4263,49 +4261,50 @@
       <c r="I37">
         <v>35</v>
       </c>
-      <c r="J37" s="4" t="s">
+      <c r="J37" t="s">
         <v>11</v>
       </c>
-      <c r="K37" s="4" t="s">
+      <c r="K37" t="s">
         <v>12</v>
       </c>
-      <c r="L37" s="4" t="s">
+      <c r="L37" t="s">
         <v>185</v>
       </c>
       <c r="M37" t="s">
         <v>181</v>
       </c>
-      <c r="N37" s="4" t="s">
+      <c r="N37" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="I38">
         <v>36</v>
       </c>
-      <c r="J38" s="4" t="s">
+      <c r="J38" t="s">
         <v>11</v>
       </c>
-      <c r="K38" s="4" t="s">
+      <c r="K38" t="s">
         <v>12</v>
       </c>
-      <c r="L38" s="4" t="s">
+      <c r="L38" t="s">
         <v>186</v>
       </c>
-      <c r="M38" s="4" t="s">
+      <c r="M38" t="s">
         <v>181</v>
       </c>
-      <c r="N38" s="4" t="s">
+      <c r="N38" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="3">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>